<commit_message>
Person count lib alpha version.
</commit_message>
<xml_diff>
--- a/Optimal_Pooling_Final_AP_Chart.xlsx
+++ b/Optimal_Pooling_Final_AP_Chart.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Object Bank 20words" sheetId="1" r:id="rId1"/>
     <sheet name="CNN 128d" sheetId="2" r:id="rId2"/>
     <sheet name="HOG+BOW" sheetId="3" r:id="rId3"/>
     <sheet name="SIFT+BOW" sheetId="4" r:id="rId4"/>
+    <sheet name="Low-level ALL" sheetId="5" r:id="rId5"/>
+    <sheet name="High-level ALL" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="121">
   <si>
     <t>Action Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -309,6 +311,170 @@
   </si>
   <si>
     <t>vgg-m-128 网络 全连接层特征 128维</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Assembling_shelter </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batting_a_run</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Making_a_cake </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOG descriptor</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIFT descriptor</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max-Pooling</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimal-Pooling</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E002 Feeding an animal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E003 Landing a fish</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E005 Wedding Ceremony</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E006 Birth party</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E007 Changing a vehicle tire</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E008 Flash mod gathering</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E009 Getting a vehicle unstuck</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E010 Grooming an animal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E011 Making a sandwich</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E012 Parade</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E013 Parkout</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E014 Reparing an appliance</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E015 Working on a sewing project</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>P001 Assembling shelter</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>P002 Batting a run</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>P003 Making a cake</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action ID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E001 Attempting an aboard trick</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E004</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E005</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E007</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E008</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E009</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E010</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E011</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E012</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E013</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E014</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E015</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>P001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>P002</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E004 Working on a woodworking project</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Object Bank 20 words</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CNN 128d </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -316,7 +482,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="#,##0.000_ "/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +542,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -392,7 +569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -400,6 +577,141 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -410,7 +722,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -425,16 +737,100 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -743,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C2" sqref="C2:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1100,17 +1496,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6">
+      <c r="B20" s="20"/>
+      <c r="C20" s="5">
         <v>0.32450000000000001</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>0.33739999999999998</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <f t="shared" si="0"/>
         <v>1.2899999999999967E-2</v>
       </c>
@@ -1118,6 +1514,96 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A24" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A25" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A27" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A30" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A31" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A32" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A33" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A34" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A37" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A38" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A39" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="11" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1134,8 +1620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1489,17 +1975,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6">
+      <c r="B20" s="21"/>
+      <c r="C20" s="5">
         <v>0.48159999999999997</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>0.48499999999999999</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <f t="shared" si="0"/>
         <v>3.4000000000000141E-3</v>
       </c>
@@ -1523,7 +2009,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C2" sqref="C2:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1827,7 +2313,7 @@
         <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="C17" s="4">
         <v>0.16159999999999999</v>
@@ -1845,7 +2331,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2">
         <v>0.37909999999999999</v>
@@ -1863,7 +2349,7 @@
         <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2">
         <v>6.5600000000000006E-2</v>
@@ -1877,19 +2363,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6">
+      <c r="B20" s="21"/>
+      <c r="C20" s="5">
         <f>AVERAGE(C2:C19)</f>
         <v>0.22639999999999999</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <f>AVERAGE(D2:D19)</f>
         <v>0.25173333333333336</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <f>D20-C20</f>
         <v>2.5333333333333374E-2</v>
       </c>
@@ -1913,7 +2399,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C2" sqref="C2:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2267,19 +2753,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6">
+      <c r="B20" s="21"/>
+      <c r="C20" s="5">
         <f>AVERAGE(C2:C19)</f>
         <v>0.16835555555555554</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <f>AVERAGE(D2:D19)</f>
         <v>0.17640555555555557</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <f>D20-C20</f>
         <v>8.0500000000000294E-3</v>
       </c>
@@ -2296,4 +2782,774 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="39.375" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="19.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="23"/>
+      <c r="B2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0.43459999999999999</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0.45710000000000001</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0.27529999999999999</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.29809999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.31969999999999998</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0.36859999999999998</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.21709999999999999</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.22339999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0.5111</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.58609999999999995</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.252</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.29420000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0.30669999999999997</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.15809999999999999</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.21740000000000001</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.18920000000000001</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.18490000000000001</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.1754</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.22009999999999999</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.13750000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0.1118</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.1016</v>
+      </c>
+      <c r="D9" s="12">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="E9" s="14">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.26929999999999998</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.32529999999999998</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0.18060000000000001</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.20130000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.3569</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.36180000000000001</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.1489</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.1802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.1356</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.17979999999999999</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.15129999999999999</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0.12509999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="12">
+        <v>7.9799999999999996E-2</v>
+      </c>
+      <c r="C13" s="13">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D13" s="12">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.1123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0.14410000000000001</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.2162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.1255</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.12970000000000001</v>
+      </c>
+      <c r="D15" s="12">
+        <v>9.1200000000000003E-2</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.10349999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.1767</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.23269999999999999</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.15429999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.1043</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0.19450000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="13">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.1472</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.1288</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.13039999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="12">
+        <v>0.37909999999999999</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.42420000000000002</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.36230000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="12">
+        <v>6.5600000000000006E-2</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.1166</v>
+      </c>
+      <c r="D20" s="12">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="E20" s="14">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="17">
+        <f>AVERAGE(B3:B20)</f>
+        <v>0.22639999999999999</v>
+      </c>
+      <c r="C21" s="18">
+        <f>AVERAGE(C3:C20)</f>
+        <v>0.25173333333333336</v>
+      </c>
+      <c r="D21" s="17">
+        <f>AVERAGE(D3:D20)</f>
+        <v>0.16835555555555554</v>
+      </c>
+      <c r="E21" s="19">
+        <f>AVERAGE(E3:E20)</f>
+        <v>0.17640555555555557</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="32.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="40.5" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
+    <col min="5" max="5" width="42.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="31"/>
+      <c r="B2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0.52659999999999996</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0.65339999999999998</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.65429999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.28249999999999997</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.38790000000000002</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.39350000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0.53049999999999997</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.56510000000000005</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.74450000000000005</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.74650000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.44369999999999998</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.4758</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.81769999999999998</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.81289999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.25019999999999998</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.25619999999999998</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.59</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.58130000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.38290000000000002</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.38390000000000002</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.38890000000000002</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.3891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.215</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.21729999999999999</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.3226</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0.33710000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.49769999999999998</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.52129999999999999</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0.4456</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.46129999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.27110000000000001</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.3029</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.62660000000000005</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.63600000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.1414</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.14269999999999999</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.26910000000000001</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.30309999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.1678</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.24909999999999999</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.31169999999999998</v>
+      </c>
+      <c r="C14" s="35">
+        <v>0.307</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.42520000000000002</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.42530000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.1467</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.15690000000000001</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.34189999999999998</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.36609999999999998</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.3805</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.38429999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.2135</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.22889999999999999</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.40960000000000002</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0.4224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="12">
+        <v>0.36130000000000001</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.36930000000000002</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.4531</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.44679999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="13">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.59330000000000005</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="E19" s="37">
+        <v>0.94899999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0.1613</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.20530000000000001</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0.2185</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.22689999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="17">
+        <v>0.32450000000000001</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.33739999999999998</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="E21" s="19">
+        <v>0.4864</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.25" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E28" s="12"/>
+      <c r="F28" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Person count, add post processing module.
</commit_message>
<xml_diff>
--- a/Optimal_Pooling_Final_AP_Chart.xlsx
+++ b/Optimal_Pooling_Final_AP_Chart.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Object Bank 20words" sheetId="1" r:id="rId1"/>
     <sheet name="CNN 128d" sheetId="2" r:id="rId2"/>
-    <sheet name="HOG+BOW" sheetId="3" r:id="rId3"/>
-    <sheet name="SIFT+BOW" sheetId="4" r:id="rId4"/>
-    <sheet name="Low-level ALL" sheetId="5" r:id="rId5"/>
-    <sheet name="High-level ALL" sheetId="6" r:id="rId6"/>
+    <sheet name="GAO 1000" sheetId="7" r:id="rId3"/>
+    <sheet name="HOG+BOW" sheetId="3" r:id="rId4"/>
+    <sheet name="SIFT+BOW" sheetId="4" r:id="rId5"/>
+    <sheet name="Low-level ALL" sheetId="5" r:id="rId6"/>
+    <sheet name="High-level ALL" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="121">
   <si>
     <t>Action Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -722,7 +723,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -780,6 +781,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -803,6 +825,9 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -811,27 +836,6 @@
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1496,10 +1500,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="5">
         <v>0.32450000000000001</v>
       </c>
@@ -1621,7 +1625,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D20"/>
+      <selection sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1975,10 +1979,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="5">
         <v>0.48159999999999997</v>
       </c>
@@ -2006,24 +2010,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="33.75" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
-    <col min="4" max="4" width="41.125" customWidth="1"/>
-    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2035,133 +2038,121 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.43459999999999999</v>
+      <c r="C2" s="1">
+        <v>0.4451</v>
       </c>
       <c r="D2" s="2">
-        <v>0.45710000000000001</v>
+        <v>0.436</v>
       </c>
       <c r="E2" s="2">
         <f>D2-C2</f>
-        <v>2.250000000000002E-2</v>
+        <v>-9.099999999999997E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>0.31969999999999998</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.36859999999999998</v>
+        <v>0.33810000000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.40250000000000002</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E19" si="0">D3-C3</f>
-        <v>4.8899999999999999E-2</v>
+        <f t="shared" ref="E3:E20" si="0">D3-C3</f>
+        <v>6.4400000000000013E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>0.5111</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.58609999999999995</v>
+        <v>0.18390000000000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.21590000000000001</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>7.4999999999999956E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4">
-        <v>0.30669999999999997</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="E5" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.1699999999999997E-2</v>
+      <c r="C5" s="2">
+        <v>0.1285</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.16839999999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9899999999999991E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.21740000000000001</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.18920000000000001</v>
-      </c>
-      <c r="E6" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.8200000000000003E-2</v>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.1754</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.22009999999999999</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>4.469999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4">
-        <v>0.1118</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.1016</v>
-      </c>
-      <c r="E8" s="4">
-        <f t="shared" si="0"/>
-        <v>-1.0200000000000001E-2</v>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -2171,15 +2162,11 @@
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2">
-        <v>0.26929999999999998</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.32529999999999998</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>5.5999999999999994E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -2189,15 +2176,11 @@
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2">
-        <v>0.3569</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.36180000000000001</v>
-      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>4.9000000000000155E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -2207,15 +2190,11 @@
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2">
-        <v>0.1356</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.17979999999999999</v>
-      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>4.4199999999999989E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -2225,15 +2204,11 @@
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2">
-        <v>7.9799999999999996E-2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>9.6000000000000002E-2</v>
-      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>1.6200000000000006E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -2243,15 +2218,11 @@
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="2">
-        <v>0.14410000000000001</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.15279999999999999</v>
-      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>8.6999999999999855E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -2261,15 +2232,11 @@
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2">
-        <v>0.1255</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.12970000000000001</v>
-      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>4.2000000000000093E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -2279,15 +2246,11 @@
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2">
-        <v>0.1767</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.23269999999999999</v>
-      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>5.5999999999999994E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -2297,33 +2260,25 @@
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="2">
-        <v>0.1043</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.15740000000000001</v>
-      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>5.3100000000000008E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.16159999999999999</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.1472</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>-1.4399999999999996E-2</v>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -2331,58 +2286,39 @@
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.37909999999999999</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.42420000000000002</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>4.5100000000000029E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="2">
-        <v>6.5600000000000006E-2</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.1166</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>5.099999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="5">
-        <f>AVERAGE(C2:C19)</f>
-        <v>0.22639999999999999</v>
-      </c>
-      <c r="D20" s="5">
-        <f>AVERAGE(D2:D19)</f>
-        <v>0.25173333333333336</v>
-      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="7">
-        <f>D20-C20</f>
-        <v>2.5333333333333374E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>77</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2391,6 +2327,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2413,145 +2350,145 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>0.27529999999999999</v>
+        <v>0.43459999999999999</v>
       </c>
       <c r="D2" s="2">
-        <v>0.29809999999999998</v>
+        <v>0.45710000000000001</v>
       </c>
       <c r="E2" s="2">
         <f>D2-C2</f>
-        <v>2.2799999999999987E-2</v>
+        <v>2.250000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>0.21709999999999999</v>
+        <v>0.31969999999999998</v>
       </c>
       <c r="D3" s="2">
-        <v>0.22339999999999999</v>
+        <v>0.36859999999999998</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E19" si="0">D3-C3</f>
-        <v>6.3E-3</v>
+        <v>4.8899999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>0.252</v>
+        <v>0.5111</v>
       </c>
       <c r="D4" s="2">
-        <v>0.29420000000000002</v>
+        <v>0.58609999999999995</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>4.2200000000000015E-2</v>
+        <v>7.4999999999999956E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4">
-        <v>0.15809999999999999</v>
+        <v>0.30669999999999997</v>
       </c>
       <c r="D5" s="4">
-        <v>0.13</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>-2.8099999999999986E-2</v>
+        <v>-2.1699999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4">
-        <v>0.18490000000000001</v>
+        <v>0.21740000000000001</v>
       </c>
       <c r="D6" s="4">
-        <v>0.16500000000000001</v>
+        <v>0.18920000000000001</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>-1.9900000000000001E-2</v>
+        <v>-2.8200000000000003E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4">
-        <v>0.14510000000000001</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.13750000000000001</v>
-      </c>
-      <c r="E7" s="4">
-        <f t="shared" si="0"/>
-        <v>-7.5999999999999956E-3</v>
+      <c r="C7" s="2">
+        <v>0.1754</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.22009999999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>4.469999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
-        <v>7.5499999999999998E-2</v>
-      </c>
-      <c r="D8" s="2">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>6.5000000000000058E-3</v>
+      <c r="C8" s="4">
+        <v>0.1118</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.1016</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.0200000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -2562,14 +2499,14 @@
         <v>12</v>
       </c>
       <c r="C9" s="2">
-        <v>0.18060000000000001</v>
+        <v>0.26929999999999998</v>
       </c>
       <c r="D9" s="2">
-        <v>0.20130000000000001</v>
+        <v>0.32529999999999998</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>2.0699999999999996E-2</v>
+        <v>5.5999999999999994E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -2580,32 +2517,32 @@
         <v>14</v>
       </c>
       <c r="C10" s="2">
-        <v>0.1489</v>
+        <v>0.3569</v>
       </c>
       <c r="D10" s="2">
-        <v>0.1802</v>
+        <v>0.36180000000000001</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>3.1299999999999994E-2</v>
+        <v>4.9000000000000155E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4">
-        <v>0.15129999999999999</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.12509999999999999</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.6200000000000001E-2</v>
+      <c r="C11" s="2">
+        <v>0.1356</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.17979999999999999</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4199999999999989E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -2616,14 +2553,14 @@
         <v>18</v>
       </c>
       <c r="C12" s="2">
-        <v>7.1300000000000002E-2</v>
+        <v>7.9799999999999996E-2</v>
       </c>
       <c r="D12" s="2">
-        <v>0.1123</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>4.0999999999999995E-2</v>
+        <v>1.6200000000000006E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -2634,14 +2571,14 @@
         <v>20</v>
       </c>
       <c r="C13" s="2">
-        <v>0.20599999999999999</v>
+        <v>0.14410000000000001</v>
       </c>
       <c r="D13" s="2">
-        <v>0.2162</v>
+        <v>0.15279999999999999</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>1.0200000000000015E-2</v>
+        <v>8.6999999999999855E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -2652,32 +2589,32 @@
         <v>22</v>
       </c>
       <c r="C14" s="2">
-        <v>9.1200000000000003E-2</v>
+        <v>0.1255</v>
       </c>
       <c r="D14" s="2">
-        <v>0.10349999999999999</v>
+        <v>0.12970000000000001</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>1.2299999999999991E-2</v>
+        <v>4.2000000000000093E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="4">
-        <v>0.17730000000000001</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.15429999999999999</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.300000000000002E-2</v>
+      <c r="C15" s="2">
+        <v>0.1767</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.23269999999999999</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5999999999999994E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -2688,50 +2625,50 @@
         <v>26</v>
       </c>
       <c r="C16" s="2">
-        <v>0.17949999999999999</v>
+        <v>0.1043</v>
       </c>
       <c r="D16" s="2">
-        <v>0.19450000000000001</v>
+        <v>0.15740000000000001</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>1.5000000000000013E-2</v>
+        <v>5.3100000000000008E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.1288</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.13039999999999999</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>1.5999999999999903E-3</v>
+      <c r="B17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.1472</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.4399999999999996E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2">
-        <v>0.34399999999999997</v>
+        <v>0.37909999999999999</v>
       </c>
       <c r="D18" s="2">
-        <v>0.36230000000000001</v>
+        <v>0.42420000000000002</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>1.8300000000000038E-2</v>
+        <v>4.5100000000000029E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -2739,35 +2676,35 @@
         <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2">
-        <v>4.3499999999999997E-2</v>
+        <v>6.5600000000000006E-2</v>
       </c>
       <c r="D19" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>0.1166</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>2.1500000000000005E-2</v>
+        <v>5.099999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="5">
         <f>AVERAGE(C2:C19)</f>
-        <v>0.16835555555555554</v>
+        <v>0.22639999999999999</v>
       </c>
       <c r="D20" s="5">
         <f>AVERAGE(D2:D19)</f>
-        <v>0.17640555555555557</v>
+        <v>0.25173333333333336</v>
       </c>
       <c r="E20" s="7">
         <f>D20-C20</f>
-        <v>8.0500000000000294E-3</v>
+        <v>2.5333333333333374E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -2785,6 +2722,396 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="33.75" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="4" max="4" width="41.125" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.27529999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.29809999999999998</v>
+      </c>
+      <c r="E2" s="2">
+        <f>D2-C2</f>
+        <v>2.2799999999999987E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.21709999999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.22339999999999999</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E19" si="0">D3-C3</f>
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.252</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2200000000000015E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.15809999999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.8099999999999986E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.18490000000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.9900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.5999999999999956E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000058E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.18060000000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.20130000000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0699999999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.1489</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.1802</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1299999999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.15129999999999999</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.12509999999999999</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.6200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.1123</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.2162</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0200000000000015E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2">
+        <v>9.1200000000000003E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2299999999999991E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.15429999999999999</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.1288</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.13039999999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999903E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.36230000000000001</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8300000000000038E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1500000000000005E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="5">
+        <f>AVERAGE(C2:C19)</f>
+        <v>0.16835555555555554</v>
+      </c>
+      <c r="D20" s="5">
+        <f>AVERAGE(D2:D19)</f>
+        <v>0.17640555555555557</v>
+      </c>
+      <c r="E20" s="7">
+        <f>D20-C20</f>
+        <v>8.0500000000000294E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A20:B20"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -2802,20 +3129,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="23"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="8" t="s">
         <v>85</v>
       </c>
@@ -3169,12 +3496,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3187,35 +3514,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="30"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="31"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="22" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="23" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="12">
@@ -3232,7 +3559,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="23" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="13">
@@ -3249,7 +3576,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12">
@@ -3266,7 +3593,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="23" t="s">
         <v>74</v>
       </c>
       <c r="B6" s="12">
@@ -3283,7 +3610,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="23" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="12">
@@ -3300,7 +3627,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="23" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="12">
@@ -3317,7 +3644,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="23" t="s">
         <v>107</v>
       </c>
       <c r="B9" s="12">
@@ -3334,7 +3661,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
       <c r="B10" s="12">
@@ -3351,7 +3678,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="23" t="s">
         <v>109</v>
       </c>
       <c r="B11" s="12">
@@ -3368,7 +3695,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="23" t="s">
         <v>110</v>
       </c>
       <c r="B12" s="12">
@@ -3385,7 +3712,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="23" t="s">
         <v>111</v>
       </c>
       <c r="B13" s="12">
@@ -3402,13 +3729,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="23" t="s">
         <v>112</v>
       </c>
       <c r="B14" s="13">
         <v>0.31169999999999998</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="24">
         <v>0.307</v>
       </c>
       <c r="D14" s="12">
@@ -3419,7 +3746,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="23" t="s">
         <v>113</v>
       </c>
       <c r="B15" s="12">
@@ -3436,7 +3763,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="23" t="s">
         <v>114</v>
       </c>
       <c r="B16" s="12">
@@ -3453,7 +3780,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="B17" s="12">
@@ -3470,7 +3797,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="12">
@@ -3487,7 +3814,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="13">
@@ -3499,12 +3826,12 @@
       <c r="D19" s="13">
         <v>0.95599999999999996</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="26">
         <v>0.94899999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="12">
@@ -3521,7 +3848,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="25" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="17">

</xml_diff>